<commit_message>
Add support for shared courses. 	Thanks Danila for pointing out! Improve documentation and readability.
</commit_message>
<xml_diff>
--- a/Build/out/Result.xlsx
+++ b/Build/out/Result.xlsx
@@ -63,7 +63,7 @@
       <sz val="10"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="16">
     <fill>
       <patternFill/>
     </fill>
@@ -131,7 +131,22 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="004285F4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="00F4B400"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="000F9D58"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="007F00FF"/>
       </patternFill>
     </fill>
   </fills>
@@ -274,7 +289,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
@@ -416,20 +431,35 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1059,13 +1089,13 @@
       <c r="E4" s="44" t="n"/>
       <c r="F4" s="50" t="inlineStr">
         <is>
-          <t>MA1 (Lec)</t>
+          <t>ITP (Lec)</t>
         </is>
       </c>
       <c r="G4" s="44" t="n"/>
       <c r="H4" s="51" t="inlineStr">
         <is>
-          <t>FSE (Lec)</t>
+          <t>DE (Lec)</t>
         </is>
       </c>
       <c r="I4" s="43" t="n"/>
@@ -1106,13 +1136,13 @@
       <c r="E5" s="44" t="n"/>
       <c r="F5" s="50" t="inlineStr">
         <is>
-          <t>Sergey Gorodetskiy</t>
+          <t>Luiz Araujo</t>
         </is>
       </c>
       <c r="G5" s="44" t="n"/>
       <c r="H5" s="51" t="inlineStr">
         <is>
-          <t>Evgeniy Bobrov</t>
+          <t>Nikolay Shilov</t>
         </is>
       </c>
       <c r="I5" s="43" t="n"/>
@@ -1198,28 +1228,20 @@
       <c r="E7" s="44" t="n"/>
       <c r="F7" s="50" t="inlineStr">
         <is>
-          <t>MA1 (Tut)</t>
+          <t>ITP (Tut)</t>
         </is>
       </c>
       <c r="G7" s="44" t="n"/>
       <c r="H7" s="53" t="inlineStr">
         <is>
-          <t>FSE (Lab)</t>
-        </is>
-      </c>
-      <c r="I7" s="3" t="n"/>
-      <c r="J7" s="53" t="inlineStr">
-        <is>
-          <t>FSE (Lab)</t>
-        </is>
-      </c>
-      <c r="K7" s="3" t="n"/>
-      <c r="L7" s="53" t="inlineStr">
-        <is>
-          <t>FSE (Lab)</t>
-        </is>
-      </c>
-      <c r="M7" s="3" t="n"/>
+          <t>DE (Tut)</t>
+        </is>
+      </c>
+      <c r="I7" s="43" t="n"/>
+      <c r="J7" s="43" t="n"/>
+      <c r="K7" s="43" t="n"/>
+      <c r="L7" s="43" t="n"/>
+      <c r="M7" s="44" t="n"/>
       <c r="N7" s="3" t="n"/>
       <c r="O7" s="3" t="n"/>
       <c r="P7" s="3" t="n"/>
@@ -1253,28 +1275,20 @@
       <c r="E8" s="44" t="n"/>
       <c r="F8" s="50" t="inlineStr">
         <is>
-          <t>Sergey Gorodetskiy</t>
+          <t>Luiz Araujo</t>
         </is>
       </c>
       <c r="G8" s="44" t="n"/>
       <c r="H8" s="53" t="inlineStr">
         <is>
-          <t>Pavel Kolychev</t>
-        </is>
-      </c>
-      <c r="I8" s="3" t="n"/>
-      <c r="J8" s="53" t="inlineStr">
-        <is>
-          <t>Nursultan Askarbekuly</t>
-        </is>
-      </c>
-      <c r="K8" s="3" t="n"/>
-      <c r="L8" s="53" t="inlineStr">
-        <is>
-          <t>Oleg Ignatov</t>
-        </is>
-      </c>
-      <c r="M8" s="3" t="n"/>
+          <t>Ivan Konyukhov</t>
+        </is>
+      </c>
+      <c r="I8" s="43" t="n"/>
+      <c r="J8" s="43" t="n"/>
+      <c r="K8" s="43" t="n"/>
+      <c r="L8" s="43" t="n"/>
+      <c r="M8" s="44" t="n"/>
       <c r="N8" s="3" t="n"/>
       <c r="O8" s="3" t="n"/>
       <c r="P8" s="3" t="n"/>
@@ -1305,21 +1319,17 @@
       <c r="D9" s="43" t="n"/>
       <c r="E9" s="44" t="n"/>
       <c r="F9" s="50" t="n">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G9" s="44" t="n"/>
       <c r="H9" s="53" t="n">
-        <v>101</v>
-      </c>
-      <c r="I9" s="3" t="n"/>
-      <c r="J9" s="53" t="n">
-        <v>102</v>
-      </c>
-      <c r="K9" s="3" t="n"/>
-      <c r="L9" s="53" t="n">
-        <v>103</v>
-      </c>
-      <c r="M9" s="3" t="n"/>
+        <v>107</v>
+      </c>
+      <c r="I9" s="43" t="n"/>
+      <c r="J9" s="43" t="n"/>
+      <c r="K9" s="43" t="n"/>
+      <c r="L9" s="43" t="n"/>
+      <c r="M9" s="44" t="n"/>
       <c r="N9" s="3" t="n"/>
       <c r="O9" s="3" t="n"/>
       <c r="P9" s="3" t="n"/>
@@ -1361,28 +1371,24 @@
       <c r="E10" s="2" t="n"/>
       <c r="F10" s="50" t="inlineStr">
         <is>
-          <t>MA1 (Lab)</t>
+          <t>ITP (Lab)</t>
         </is>
       </c>
       <c r="G10" s="1" t="n"/>
-      <c r="H10" s="10" t="n"/>
-      <c r="I10" s="51" t="inlineStr">
-        <is>
-          <t>FSE (Lab)</t>
-        </is>
-      </c>
-      <c r="J10" s="3" t="n"/>
-      <c r="K10" s="51" t="inlineStr">
-        <is>
-          <t>FSE (Lab)</t>
-        </is>
-      </c>
+      <c r="H10" s="55" t="inlineStr">
+        <is>
+          <t>DE (Lab)</t>
+        </is>
+      </c>
+      <c r="I10" s="1" t="n"/>
+      <c r="J10" s="53" t="inlineStr">
+        <is>
+          <t>DE (Lab)</t>
+        </is>
+      </c>
+      <c r="K10" s="1" t="n"/>
       <c r="L10" s="1" t="n"/>
-      <c r="M10" s="51" t="inlineStr">
-        <is>
-          <t>FSE (Lab)</t>
-        </is>
-      </c>
+      <c r="M10" s="1" t="n"/>
       <c r="N10" s="1" t="n"/>
       <c r="O10" s="1" t="n"/>
       <c r="P10" s="1" t="n"/>
@@ -1420,28 +1426,24 @@
       <c r="E11" s="2" t="n"/>
       <c r="F11" s="50" t="inlineStr">
         <is>
-          <t>Pavel Khakimov</t>
+          <t>Munir Makhmutov</t>
         </is>
       </c>
       <c r="G11" s="1" t="n"/>
-      <c r="H11" s="1" t="n"/>
-      <c r="I11" s="51" t="inlineStr">
-        <is>
-          <t>Pavel Kolychev</t>
-        </is>
-      </c>
-      <c r="J11" s="3" t="n"/>
-      <c r="K11" s="51" t="inlineStr">
-        <is>
-          <t>Nursultan Askarbekuly</t>
-        </is>
-      </c>
+      <c r="H11" s="51" t="inlineStr">
+        <is>
+          <t>Marat Mingazov</t>
+        </is>
+      </c>
+      <c r="I11" s="1" t="n"/>
+      <c r="J11" s="53" t="inlineStr">
+        <is>
+          <t>Victor Kazorin</t>
+        </is>
+      </c>
+      <c r="K11" s="1" t="n"/>
       <c r="L11" s="1" t="n"/>
-      <c r="M11" s="53" t="inlineStr">
-        <is>
-          <t>Oleg Ignatov</t>
-        </is>
-      </c>
+      <c r="M11" s="3" t="n"/>
       <c r="N11" s="1" t="n"/>
       <c r="O11" s="1" t="n"/>
       <c r="P11" s="1" t="n"/>
@@ -1473,22 +1475,20 @@
         <v>102</v>
       </c>
       <c r="E12" s="2" t="n"/>
-      <c r="F12" s="55" t="n">
-        <v>301</v>
+      <c r="F12" s="56" t="n">
+        <v>300</v>
       </c>
       <c r="G12" s="3" t="n"/>
-      <c r="H12" s="1" t="n"/>
-      <c r="I12" s="51" t="n">
+      <c r="H12" s="51" t="n">
         <v>103</v>
       </c>
-      <c r="J12" s="3" t="n"/>
-      <c r="K12" s="51" t="n">
+      <c r="I12" s="1" t="n"/>
+      <c r="J12" s="53" t="n">
         <v>104</v>
       </c>
+      <c r="K12" s="1" t="n"/>
       <c r="L12" s="1" t="n"/>
-      <c r="M12" s="53" t="n">
-        <v>300</v>
-      </c>
+      <c r="M12" s="3" t="n"/>
       <c r="N12" s="1" t="n"/>
       <c r="O12" s="1" t="n"/>
       <c r="P12" s="1" t="n"/>
@@ -1531,13 +1531,21 @@
       <c r="F13" s="1" t="n"/>
       <c r="G13" s="50" t="inlineStr">
         <is>
-          <t>MA1 (Lab)</t>
+          <t>ITP (Lab)</t>
         </is>
       </c>
       <c r="H13" s="1" t="n"/>
-      <c r="I13" s="3" t="n"/>
+      <c r="I13" s="53" t="inlineStr">
+        <is>
+          <t>DE (Lab)</t>
+        </is>
+      </c>
       <c r="J13" s="1" t="n"/>
-      <c r="K13" s="3" t="n"/>
+      <c r="K13" s="53" t="inlineStr">
+        <is>
+          <t>DE (Lab)</t>
+        </is>
+      </c>
       <c r="L13" s="1" t="n"/>
       <c r="M13" s="3" t="n"/>
       <c r="N13" s="1" t="n"/>
@@ -1564,27 +1572,35 @@
     <row r="14">
       <c r="A14" s="52" t="n"/>
       <c r="B14" s="6" t="n"/>
-      <c r="C14" s="55" t="inlineStr">
+      <c r="C14" s="56" t="inlineStr">
         <is>
           <t>Anastasiya Puzankova</t>
         </is>
       </c>
       <c r="D14" s="3" t="n"/>
-      <c r="E14" s="55" t="inlineStr">
+      <c r="E14" s="56" t="inlineStr">
         <is>
           <t>Oleg Bulichev</t>
         </is>
       </c>
       <c r="F14" s="3" t="n"/>
-      <c r="G14" s="55" t="inlineStr">
-        <is>
-          <t>Pavel Khakimov</t>
+      <c r="G14" s="56" t="inlineStr">
+        <is>
+          <t>Munir Makhmutov</t>
         </is>
       </c>
       <c r="H14" s="1" t="n"/>
-      <c r="I14" s="3" t="n"/>
+      <c r="I14" s="53" t="inlineStr">
+        <is>
+          <t>Marat Mingazov</t>
+        </is>
+      </c>
       <c r="J14" s="1" t="n"/>
-      <c r="K14" s="3" t="n"/>
+      <c r="K14" s="53" t="inlineStr">
+        <is>
+          <t>Victor Kazorin</t>
+        </is>
+      </c>
       <c r="L14" s="1" t="n"/>
       <c r="M14" s="3" t="n"/>
       <c r="N14" s="1" t="n"/>
@@ -1620,12 +1636,16 @@
       </c>
       <c r="F15" s="1" t="n"/>
       <c r="G15" s="50" t="n">
+        <v>300</v>
+      </c>
+      <c r="H15" s="1" t="n"/>
+      <c r="I15" s="53" t="n">
         <v>103</v>
       </c>
-      <c r="H15" s="1" t="n"/>
-      <c r="I15" s="3" t="n"/>
       <c r="J15" s="1" t="n"/>
-      <c r="K15" s="3" t="n"/>
+      <c r="K15" s="53" t="n">
+        <v>104</v>
+      </c>
       <c r="L15" s="1" t="n"/>
       <c r="M15" s="3" t="n"/>
       <c r="N15" s="1" t="n"/>
@@ -2053,21 +2073,25 @@
         </is>
       </c>
       <c r="G26" s="44" t="n"/>
-      <c r="H26" s="51" t="inlineStr">
-        <is>
-          <t>OS (Lec)</t>
-        </is>
-      </c>
-      <c r="I26" s="43" t="n"/>
-      <c r="J26" s="43" t="n"/>
-      <c r="K26" s="43" t="n"/>
-      <c r="L26" s="43" t="n"/>
-      <c r="M26" s="44" t="n"/>
-      <c r="N26" s="3" t="n"/>
-      <c r="O26" s="3" t="n"/>
-      <c r="P26" s="3" t="n"/>
-      <c r="Q26" s="3" t="n"/>
-      <c r="R26" s="3" t="n"/>
+      <c r="H26" s="1" t="n"/>
+      <c r="I26" s="1" t="n"/>
+      <c r="J26" s="1" t="n"/>
+      <c r="K26" s="1" t="n"/>
+      <c r="L26" s="51" t="inlineStr">
+        <is>
+          <t>DE (Lab)</t>
+        </is>
+      </c>
+      <c r="M26" s="1" t="n"/>
+      <c r="N26" s="57" t="inlineStr">
+        <is>
+          <t>DS (Lec)</t>
+        </is>
+      </c>
+      <c r="O26" s="43" t="n"/>
+      <c r="P26" s="43" t="n"/>
+      <c r="Q26" s="43" t="n"/>
+      <c r="R26" s="44" t="n"/>
       <c r="S26" s="3" t="n"/>
       <c r="T26" s="3" t="n"/>
       <c r="U26" s="3" t="n"/>
@@ -2108,21 +2132,25 @@
         </is>
       </c>
       <c r="G27" s="44" t="n"/>
-      <c r="H27" s="51" t="inlineStr">
-        <is>
-          <t>Giancarlo Succi</t>
-        </is>
-      </c>
-      <c r="I27" s="43" t="n"/>
-      <c r="J27" s="43" t="n"/>
-      <c r="K27" s="43" t="n"/>
-      <c r="L27" s="43" t="n"/>
-      <c r="M27" s="44" t="n"/>
-      <c r="N27" s="3" t="n"/>
-      <c r="O27" s="3" t="n"/>
-      <c r="P27" s="3" t="n"/>
-      <c r="Q27" s="3" t="n"/>
-      <c r="R27" s="3" t="n"/>
+      <c r="H27" s="1" t="n"/>
+      <c r="I27" s="1" t="n"/>
+      <c r="J27" s="1" t="n"/>
+      <c r="K27" s="1" t="n"/>
+      <c r="L27" s="51" t="inlineStr">
+        <is>
+          <t>Marat Mingazov</t>
+        </is>
+      </c>
+      <c r="M27" s="1" t="n"/>
+      <c r="N27" s="57" t="inlineStr">
+        <is>
+          <t>Ahsan Kazmi</t>
+        </is>
+      </c>
+      <c r="O27" s="43" t="n"/>
+      <c r="P27" s="43" t="n"/>
+      <c r="Q27" s="43" t="n"/>
+      <c r="R27" s="44" t="n"/>
       <c r="S27" s="3" t="n"/>
       <c r="T27" s="4" t="n"/>
       <c r="U27" s="4" t="n"/>
@@ -2142,32 +2170,34 @@
     <row r="28">
       <c r="A28" s="48" t="n"/>
       <c r="B28" s="49" t="n">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C28" s="1" t="n"/>
       <c r="D28" s="50" t="n">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E28" s="50" t="n">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F28" s="50" t="n">
         <v>108</v>
       </c>
       <c r="G28" s="44" t="n"/>
-      <c r="H28" s="51" t="n">
+      <c r="H28" s="1" t="n"/>
+      <c r="I28" s="1" t="n"/>
+      <c r="J28" s="1" t="n"/>
+      <c r="K28" s="1" t="n"/>
+      <c r="L28" s="51" t="n">
+        <v>101</v>
+      </c>
+      <c r="M28" s="1" t="n"/>
+      <c r="N28" s="57" t="n">
         <v>107</v>
       </c>
-      <c r="I28" s="43" t="n"/>
-      <c r="J28" s="43" t="n"/>
-      <c r="K28" s="43" t="n"/>
-      <c r="L28" s="43" t="n"/>
-      <c r="M28" s="44" t="n"/>
-      <c r="N28" s="3" t="n"/>
-      <c r="O28" s="3" t="n"/>
-      <c r="P28" s="3" t="n"/>
-      <c r="Q28" s="3" t="n"/>
-      <c r="R28" s="3" t="n"/>
+      <c r="O28" s="43" t="n"/>
+      <c r="P28" s="43" t="n"/>
+      <c r="Q28" s="43" t="n"/>
+      <c r="R28" s="44" t="n"/>
       <c r="S28" s="3" t="n"/>
       <c r="T28" s="3" t="n"/>
       <c r="U28" s="3" t="n"/>
@@ -2204,16 +2234,16 @@
         </is>
       </c>
       <c r="G29" s="44" t="n"/>
-      <c r="H29" s="53" t="inlineStr">
-        <is>
-          <t>OS (Tut)</t>
-        </is>
-      </c>
-      <c r="I29" s="43" t="n"/>
-      <c r="J29" s="43" t="n"/>
-      <c r="K29" s="43" t="n"/>
-      <c r="L29" s="43" t="n"/>
-      <c r="M29" s="44" t="n"/>
+      <c r="H29" s="3" t="n"/>
+      <c r="I29" s="3" t="n"/>
+      <c r="J29" s="3" t="n"/>
+      <c r="K29" s="3" t="n"/>
+      <c r="L29" s="3" t="n"/>
+      <c r="M29" s="53" t="inlineStr">
+        <is>
+          <t>DE (Lab)</t>
+        </is>
+      </c>
       <c r="N29" s="3" t="n"/>
       <c r="O29" s="3" t="n"/>
       <c r="P29" s="3" t="n"/>
@@ -2251,16 +2281,16 @@
         </is>
       </c>
       <c r="G30" s="44" t="n"/>
-      <c r="H30" s="53" t="inlineStr">
-        <is>
-          <t>Nikita Lozhnikov</t>
-        </is>
-      </c>
-      <c r="I30" s="43" t="n"/>
-      <c r="J30" s="43" t="n"/>
-      <c r="K30" s="43" t="n"/>
-      <c r="L30" s="43" t="n"/>
-      <c r="M30" s="44" t="n"/>
+      <c r="H30" s="3" t="n"/>
+      <c r="I30" s="3" t="n"/>
+      <c r="J30" s="3" t="n"/>
+      <c r="K30" s="3" t="n"/>
+      <c r="L30" s="3" t="n"/>
+      <c r="M30" s="53" t="inlineStr">
+        <is>
+          <t>Marat Mingazov</t>
+        </is>
+      </c>
       <c r="N30" s="3" t="n"/>
       <c r="O30" s="3" t="n"/>
       <c r="P30" s="3" t="n"/>
@@ -2285,8 +2315,8 @@
     <row r="31">
       <c r="A31" s="48" t="n"/>
       <c r="B31" s="6" t="n"/>
-      <c r="C31" s="55" t="n">
-        <v>101</v>
+      <c r="C31" s="56" t="n">
+        <v>102</v>
       </c>
       <c r="D31" s="1" t="n"/>
       <c r="E31" s="1" t="n"/>
@@ -2294,14 +2324,14 @@
         <v>108</v>
       </c>
       <c r="G31" s="44" t="n"/>
-      <c r="H31" s="53" t="n">
-        <v>107</v>
-      </c>
-      <c r="I31" s="43" t="n"/>
-      <c r="J31" s="43" t="n"/>
-      <c r="K31" s="43" t="n"/>
-      <c r="L31" s="43" t="n"/>
-      <c r="M31" s="44" t="n"/>
+      <c r="H31" s="3" t="n"/>
+      <c r="I31" s="3" t="n"/>
+      <c r="J31" s="3" t="n"/>
+      <c r="K31" s="3" t="n"/>
+      <c r="L31" s="3" t="n"/>
+      <c r="M31" s="53" t="n">
+        <v>101</v>
+      </c>
       <c r="N31" s="3" t="n"/>
       <c r="O31" s="3" t="n"/>
       <c r="P31" s="3" t="n"/>
@@ -2347,24 +2377,16 @@
           <t>FP (Lab)</t>
         </is>
       </c>
-      <c r="H32" s="56" t="inlineStr">
-        <is>
-          <t>OS (Lab)</t>
-        </is>
-      </c>
-      <c r="I32" s="1" t="n"/>
-      <c r="J32" s="53" t="inlineStr">
-        <is>
-          <t>OS (Lab)</t>
-        </is>
-      </c>
-      <c r="K32" s="1" t="n"/>
-      <c r="L32" s="51" t="inlineStr">
-        <is>
-          <t>OS (Lab)</t>
-        </is>
-      </c>
-      <c r="M32" s="1" t="n"/>
+      <c r="H32" s="55" t="inlineStr">
+        <is>
+          <t>PS (Lec)</t>
+        </is>
+      </c>
+      <c r="I32" s="43" t="n"/>
+      <c r="J32" s="43" t="n"/>
+      <c r="K32" s="43" t="n"/>
+      <c r="L32" s="43" t="n"/>
+      <c r="M32" s="44" t="n"/>
       <c r="N32" s="1" t="n"/>
       <c r="O32" s="1" t="n"/>
       <c r="P32" s="1" t="n"/>
@@ -2408,22 +2430,14 @@
       </c>
       <c r="H33" s="51" t="inlineStr">
         <is>
-          <t>Nikita Lozhnikov</t>
-        </is>
-      </c>
-      <c r="I33" s="1" t="n"/>
-      <c r="J33" s="53" t="inlineStr">
-        <is>
-          <t>Xavier Vasquez</t>
-        </is>
-      </c>
-      <c r="K33" s="1" t="n"/>
-      <c r="L33" s="51" t="inlineStr">
-        <is>
-          <t>Shokhista Ergasheva</t>
-        </is>
-      </c>
-      <c r="M33" s="3" t="n"/>
+          <t>Sergey Gorodetskiy</t>
+        </is>
+      </c>
+      <c r="I33" s="43" t="n"/>
+      <c r="J33" s="43" t="n"/>
+      <c r="K33" s="43" t="n"/>
+      <c r="L33" s="43" t="n"/>
+      <c r="M33" s="44" t="n"/>
       <c r="N33" s="1" t="n"/>
       <c r="O33" s="1" t="n"/>
       <c r="P33" s="1" t="n"/>
@@ -2448,29 +2462,25 @@
     <row r="34">
       <c r="A34" s="48" t="n"/>
       <c r="B34" s="49" t="n">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C34" s="43" t="n"/>
       <c r="D34" s="43" t="n"/>
       <c r="E34" s="44" t="n"/>
-      <c r="F34" s="55" t="n">
+      <c r="F34" s="56" t="n">
         <v>101</v>
       </c>
-      <c r="G34" s="55" t="n">
+      <c r="G34" s="56" t="n">
         <v>102</v>
       </c>
       <c r="H34" s="51" t="n">
-        <v>103</v>
-      </c>
-      <c r="I34" s="1" t="n"/>
-      <c r="J34" s="53" t="n">
-        <v>104</v>
-      </c>
-      <c r="K34" s="1" t="n"/>
-      <c r="L34" s="51" t="n">
-        <v>300</v>
-      </c>
-      <c r="M34" s="3" t="n"/>
+        <v>108</v>
+      </c>
+      <c r="I34" s="43" t="n"/>
+      <c r="J34" s="43" t="n"/>
+      <c r="K34" s="43" t="n"/>
+      <c r="L34" s="43" t="n"/>
+      <c r="M34" s="44" t="n"/>
       <c r="N34" s="1" t="n"/>
       <c r="O34" s="1" t="n"/>
       <c r="P34" s="1" t="n"/>
@@ -2516,24 +2526,16 @@
           <t>AGLA (Lab)</t>
         </is>
       </c>
-      <c r="H35" s="1" t="n"/>
-      <c r="I35" s="53" t="inlineStr">
-        <is>
-          <t>OS (Lab)</t>
-        </is>
-      </c>
-      <c r="J35" s="1" t="n"/>
-      <c r="K35" s="53" t="inlineStr">
-        <is>
-          <t>OS (Lab)</t>
-        </is>
-      </c>
-      <c r="L35" s="1" t="n"/>
-      <c r="M35" s="53" t="inlineStr">
-        <is>
-          <t>OS (Lab)</t>
-        </is>
-      </c>
+      <c r="H35" s="51" t="inlineStr">
+        <is>
+          <t>PS (Tut)</t>
+        </is>
+      </c>
+      <c r="I35" s="43" t="n"/>
+      <c r="J35" s="43" t="n"/>
+      <c r="K35" s="43" t="n"/>
+      <c r="L35" s="43" t="n"/>
+      <c r="M35" s="44" t="n"/>
       <c r="N35" s="1" t="n"/>
       <c r="O35" s="1" t="n"/>
       <c r="P35" s="1" t="n"/>
@@ -2565,34 +2567,26 @@
       <c r="C36" s="43" t="n"/>
       <c r="D36" s="43" t="n"/>
       <c r="E36" s="44" t="n"/>
-      <c r="F36" s="55" t="inlineStr">
+      <c r="F36" s="56" t="inlineStr">
         <is>
           <t>Timur Fayzrakhmanov</t>
         </is>
       </c>
-      <c r="G36" s="55" t="inlineStr">
+      <c r="G36" s="56" t="inlineStr">
         <is>
           <t>Nikolay Kudasov</t>
         </is>
       </c>
-      <c r="H36" s="1" t="n"/>
-      <c r="I36" s="53" t="inlineStr">
-        <is>
-          <t>Nikita Lozhnikov</t>
-        </is>
-      </c>
-      <c r="J36" s="1" t="n"/>
-      <c r="K36" s="53" t="inlineStr">
-        <is>
-          <t>Xavier Vasquez</t>
-        </is>
-      </c>
-      <c r="L36" s="1" t="n"/>
-      <c r="M36" s="53" t="inlineStr">
-        <is>
-          <t>Shokhista Ergasheva</t>
-        </is>
-      </c>
+      <c r="H36" s="51" t="inlineStr">
+        <is>
+          <t>Sergey Gorodetskiy</t>
+        </is>
+      </c>
+      <c r="I36" s="43" t="n"/>
+      <c r="J36" s="43" t="n"/>
+      <c r="K36" s="43" t="n"/>
+      <c r="L36" s="43" t="n"/>
+      <c r="M36" s="44" t="n"/>
       <c r="N36" s="1" t="n"/>
       <c r="O36" s="1" t="n"/>
       <c r="P36" s="1" t="n"/>
@@ -2617,7 +2611,7 @@
     <row r="37">
       <c r="A37" s="48" t="n"/>
       <c r="B37" s="49" t="n">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C37" s="43" t="n"/>
       <c r="D37" s="43" t="n"/>
@@ -2628,18 +2622,14 @@
       <c r="G37" s="50" t="n">
         <v>101</v>
       </c>
-      <c r="H37" s="1" t="n"/>
-      <c r="I37" s="53" t="n">
-        <v>103</v>
-      </c>
-      <c r="J37" s="1" t="n"/>
-      <c r="K37" s="53" t="n">
-        <v>104</v>
-      </c>
-      <c r="L37" s="1" t="n"/>
-      <c r="M37" s="53" t="n">
-        <v>300</v>
-      </c>
+      <c r="H37" s="51" t="n">
+        <v>108</v>
+      </c>
+      <c r="I37" s="43" t="n"/>
+      <c r="J37" s="43" t="n"/>
+      <c r="K37" s="43" t="n"/>
+      <c r="L37" s="43" t="n"/>
+      <c r="M37" s="44" t="n"/>
       <c r="N37" s="1" t="n"/>
       <c r="O37" s="1" t="n"/>
       <c r="P37" s="1" t="n"/>
@@ -3043,13 +3033,13 @@
       <c r="E48" s="44" t="n"/>
       <c r="F48" s="50" t="inlineStr">
         <is>
-          <t>ITP (Lec)</t>
+          <t>MA1 (Lec)</t>
         </is>
       </c>
       <c r="G48" s="44" t="n"/>
       <c r="H48" s="51" t="inlineStr">
         <is>
-          <t>PS (Lec)</t>
+          <t>FSE (Lec)</t>
         </is>
       </c>
       <c r="I48" s="43" t="n"/>
@@ -3069,8 +3059,12 @@
       <c r="W48" s="1" t="n"/>
       <c r="X48" s="1" t="n"/>
       <c r="Y48" s="1" t="n"/>
-      <c r="Z48" s="1" t="n"/>
-      <c r="AA48" s="1" t="n"/>
+      <c r="Z48" s="58" t="inlineStr">
+        <is>
+          <t>EM (Lec)</t>
+        </is>
+      </c>
+      <c r="AA48" s="44" t="n"/>
       <c r="AB48" s="1" t="n"/>
       <c r="AC48" s="1" t="n"/>
       <c r="AD48" s="2" t="n"/>
@@ -3090,13 +3084,13 @@
       <c r="E49" s="44" t="n"/>
       <c r="F49" s="50" t="inlineStr">
         <is>
-          <t>Luiz Araujo</t>
+          <t>Sergey Gorodetskiy</t>
         </is>
       </c>
       <c r="G49" s="44" t="n"/>
       <c r="H49" s="51" t="inlineStr">
         <is>
-          <t>Sergey Gorodetskiy</t>
+          <t>Evgeniy Bobrov</t>
         </is>
       </c>
       <c r="I49" s="43" t="n"/>
@@ -3116,8 +3110,12 @@
       <c r="W49" s="1" t="n"/>
       <c r="X49" s="1" t="n"/>
       <c r="Y49" s="1" t="n"/>
-      <c r="Z49" s="1" t="n"/>
-      <c r="AA49" s="1" t="n"/>
+      <c r="Z49" s="58" t="inlineStr">
+        <is>
+          <t>Giancarlo Succi</t>
+        </is>
+      </c>
+      <c r="AA49" s="44" t="n"/>
       <c r="AB49" s="1" t="n"/>
       <c r="AC49" s="1" t="n"/>
       <c r="AD49" s="2" t="n"/>
@@ -3134,7 +3132,7 @@
       <c r="D50" s="43" t="n"/>
       <c r="E50" s="44" t="n"/>
       <c r="F50" s="50" t="n">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G50" s="44" t="n"/>
       <c r="H50" s="51" t="n">
@@ -3157,8 +3155,10 @@
       <c r="W50" s="1" t="n"/>
       <c r="X50" s="1" t="n"/>
       <c r="Y50" s="1" t="n"/>
-      <c r="Z50" s="1" t="n"/>
-      <c r="AA50" s="1" t="n"/>
+      <c r="Z50" s="58" t="n">
+        <v>107</v>
+      </c>
+      <c r="AA50" s="44" t="n"/>
       <c r="AB50" s="1" t="n"/>
       <c r="AC50" s="1" t="n"/>
       <c r="AD50" s="2" t="n"/>
@@ -3182,20 +3182,36 @@
       <c r="E51" s="44" t="n"/>
       <c r="F51" s="50" t="inlineStr">
         <is>
-          <t>ITP (Tut)</t>
+          <t>MA1 (Tut)</t>
         </is>
       </c>
       <c r="G51" s="44" t="n"/>
       <c r="H51" s="53" t="inlineStr">
         <is>
-          <t>PS (Tut)</t>
-        </is>
-      </c>
-      <c r="I51" s="43" t="n"/>
-      <c r="J51" s="43" t="n"/>
-      <c r="K51" s="43" t="n"/>
-      <c r="L51" s="43" t="n"/>
-      <c r="M51" s="44" t="n"/>
+          <t>FSE (Lab)</t>
+        </is>
+      </c>
+      <c r="I51" s="53" t="inlineStr">
+        <is>
+          <t>PS (Lab)</t>
+        </is>
+      </c>
+      <c r="J51" s="53" t="inlineStr">
+        <is>
+          <t>FSE (Lab)</t>
+        </is>
+      </c>
+      <c r="K51" s="3" t="n"/>
+      <c r="L51" s="53" t="inlineStr">
+        <is>
+          <t>FSE (Lab)</t>
+        </is>
+      </c>
+      <c r="M51" s="53" t="inlineStr">
+        <is>
+          <t>PS (Lab)</t>
+        </is>
+      </c>
       <c r="N51" s="3" t="n"/>
       <c r="O51" s="3" t="n"/>
       <c r="P51" s="3" t="n"/>
@@ -3229,20 +3245,36 @@
       <c r="E52" s="44" t="n"/>
       <c r="F52" s="50" t="inlineStr">
         <is>
-          <t>Luiz Araujo</t>
+          <t>Sergey Gorodetskiy</t>
         </is>
       </c>
       <c r="G52" s="44" t="n"/>
       <c r="H52" s="53" t="inlineStr">
         <is>
-          <t>Sergey Gorodetskiy</t>
-        </is>
-      </c>
-      <c r="I52" s="43" t="n"/>
-      <c r="J52" s="43" t="n"/>
-      <c r="K52" s="43" t="n"/>
-      <c r="L52" s="43" t="n"/>
-      <c r="M52" s="44" t="n"/>
+          <t>Pavel Kolychev</t>
+        </is>
+      </c>
+      <c r="I52" s="53" t="inlineStr">
+        <is>
+          <t>Alexey Shikulin</t>
+        </is>
+      </c>
+      <c r="J52" s="53" t="inlineStr">
+        <is>
+          <t>Nursultan Askarbekuly</t>
+        </is>
+      </c>
+      <c r="K52" s="3" t="n"/>
+      <c r="L52" s="53" t="inlineStr">
+        <is>
+          <t>Oleg Ignatov</t>
+        </is>
+      </c>
+      <c r="M52" s="53" t="inlineStr">
+        <is>
+          <t>Azat Gaitudinov</t>
+        </is>
+      </c>
       <c r="N52" s="3" t="n"/>
       <c r="O52" s="3" t="n"/>
       <c r="P52" s="3" t="n"/>
@@ -3277,13 +3309,21 @@
       </c>
       <c r="G53" s="44" t="n"/>
       <c r="H53" s="53" t="n">
-        <v>106</v>
-      </c>
-      <c r="I53" s="43" t="n"/>
-      <c r="J53" s="43" t="n"/>
-      <c r="K53" s="43" t="n"/>
-      <c r="L53" s="43" t="n"/>
-      <c r="M53" s="44" t="n"/>
+        <v>101</v>
+      </c>
+      <c r="I53" s="53" t="n">
+        <v>104</v>
+      </c>
+      <c r="J53" s="53" t="n">
+        <v>102</v>
+      </c>
+      <c r="K53" s="3" t="n"/>
+      <c r="L53" s="53" t="n">
+        <v>103</v>
+      </c>
+      <c r="M53" s="53" t="n">
+        <v>300</v>
+      </c>
       <c r="N53" s="3" t="n"/>
       <c r="O53" s="3" t="n"/>
       <c r="P53" s="3" t="n"/>
@@ -3333,26 +3373,34 @@
       </c>
       <c r="F54" s="50" t="inlineStr">
         <is>
-          <t>ITP (Lab)</t>
+          <t>MA1 (Lab)</t>
         </is>
       </c>
       <c r="G54" s="1" t="n"/>
-      <c r="H54" s="56" t="inlineStr">
+      <c r="H54" s="55" t="inlineStr">
         <is>
           <t>PS (Lab)</t>
         </is>
       </c>
       <c r="I54" s="51" t="inlineStr">
         <is>
+          <t>FSE (Lab)</t>
+        </is>
+      </c>
+      <c r="J54" s="53" t="inlineStr">
+        <is>
           <t>PS (Lab)</t>
         </is>
       </c>
-      <c r="J54" s="3" t="n"/>
-      <c r="K54" s="1" t="n"/>
+      <c r="K54" s="51" t="inlineStr">
+        <is>
+          <t>FSE (Lab)</t>
+        </is>
+      </c>
       <c r="L54" s="1" t="n"/>
       <c r="M54" s="51" t="inlineStr">
         <is>
-          <t>PS (Lab)</t>
+          <t>FSE (Lab)</t>
         </is>
       </c>
       <c r="N54" s="1" t="n"/>
@@ -3400,7 +3448,7 @@
       </c>
       <c r="F55" s="50" t="inlineStr">
         <is>
-          <t>Munir Makhmutov</t>
+          <t>Pavel Khakimov</t>
         </is>
       </c>
       <c r="G55" s="1" t="n"/>
@@ -3411,15 +3459,23 @@
       </c>
       <c r="I55" s="51" t="inlineStr">
         <is>
+          <t>Pavel Kolychev</t>
+        </is>
+      </c>
+      <c r="J55" s="53" t="inlineStr">
+        <is>
           <t>Alexey Shikulin</t>
         </is>
       </c>
-      <c r="J55" s="3" t="n"/>
-      <c r="K55" s="1" t="n"/>
+      <c r="K55" s="51" t="inlineStr">
+        <is>
+          <t>Nursultan Askarbekuly</t>
+        </is>
+      </c>
       <c r="L55" s="1" t="n"/>
       <c r="M55" s="53" t="inlineStr">
         <is>
-          <t>Azat Gaitudinov</t>
+          <t>Oleg Ignatov</t>
         </is>
       </c>
       <c r="N55" s="1" t="n"/>
@@ -3449,29 +3505,33 @@
         <v>101</v>
       </c>
       <c r="C56" s="50" t="n">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="D56" s="50" t="n">
         <v>102</v>
       </c>
       <c r="E56" s="50" t="n">
-        <v>303</v>
-      </c>
-      <c r="F56" s="55" t="n">
-        <v>103</v>
+        <v>305</v>
+      </c>
+      <c r="F56" s="56" t="n">
+        <v>301</v>
       </c>
       <c r="G56" s="3" t="n"/>
       <c r="H56" s="51" t="n">
+        <v>302</v>
+      </c>
+      <c r="I56" s="51" t="n">
+        <v>103</v>
+      </c>
+      <c r="J56" s="53" t="n">
+        <v>303</v>
+      </c>
+      <c r="K56" s="51" t="n">
         <v>104</v>
       </c>
-      <c r="I56" s="51" t="n">
-        <v>300</v>
-      </c>
-      <c r="J56" s="3" t="n"/>
-      <c r="K56" s="1" t="n"/>
       <c r="L56" s="1" t="n"/>
       <c r="M56" s="53" t="n">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="N56" s="1" t="n"/>
       <c r="O56" s="1" t="n"/>
@@ -3523,17 +3583,17 @@
       <c r="F57" s="1" t="n"/>
       <c r="G57" s="50" t="inlineStr">
         <is>
-          <t>ITP (Lab)</t>
+          <t>MA1 (Lab)</t>
         </is>
       </c>
       <c r="H57" s="1" t="n"/>
       <c r="I57" s="3" t="n"/>
-      <c r="J57" s="51" t="inlineStr">
+      <c r="J57" s="1" t="n"/>
+      <c r="K57" s="53" t="inlineStr">
         <is>
           <t>PS (Lab)</t>
         </is>
       </c>
-      <c r="K57" s="3" t="n"/>
       <c r="L57" s="1" t="n"/>
       <c r="M57" s="3" t="n"/>
       <c r="N57" s="1" t="n"/>
@@ -3564,35 +3624,35 @@
           <t>Sirojiddin Komolov</t>
         </is>
       </c>
-      <c r="C58" s="55" t="inlineStr">
+      <c r="C58" s="56" t="inlineStr">
         <is>
           <t>Ivan Konyukhov</t>
         </is>
       </c>
-      <c r="D58" s="55" t="inlineStr">
+      <c r="D58" s="56" t="inlineStr">
         <is>
           <t>Mansur Khazeev</t>
         </is>
       </c>
-      <c r="E58" s="55" t="inlineStr">
+      <c r="E58" s="56" t="inlineStr">
         <is>
           <t>Ramil Dautov</t>
         </is>
       </c>
       <c r="F58" s="3" t="n"/>
-      <c r="G58" s="55" t="inlineStr">
-        <is>
-          <t>Munir Makhmutov</t>
+      <c r="G58" s="56" t="inlineStr">
+        <is>
+          <t>Pavel Khakimov</t>
         </is>
       </c>
       <c r="H58" s="1" t="n"/>
       <c r="I58" s="3" t="n"/>
-      <c r="J58" s="51" t="inlineStr">
+      <c r="J58" s="1" t="n"/>
+      <c r="K58" s="53" t="inlineStr">
         <is>
           <t>Alexey Shikulin</t>
         </is>
       </c>
-      <c r="K58" s="3" t="n"/>
       <c r="L58" s="1" t="n"/>
       <c r="M58" s="3" t="n"/>
       <c r="N58" s="1" t="n"/>
@@ -3636,10 +3696,10 @@
       </c>
       <c r="H59" s="1" t="n"/>
       <c r="I59" s="3" t="n"/>
-      <c r="J59" s="51" t="n">
+      <c r="J59" s="1" t="n"/>
+      <c r="K59" s="53" t="n">
         <v>104</v>
       </c>
-      <c r="K59" s="3" t="n"/>
       <c r="L59" s="1" t="n"/>
       <c r="M59" s="3" t="n"/>
       <c r="N59" s="1" t="n"/>
@@ -4047,7 +4107,7 @@
       <c r="G70" s="44" t="n"/>
       <c r="H70" s="51" t="inlineStr">
         <is>
-          <t>PM (Lec)</t>
+          <t>OS (Lec)</t>
         </is>
       </c>
       <c r="I70" s="43" t="n"/>
@@ -4063,9 +4123,13 @@
       <c r="S70" s="3" t="n"/>
       <c r="T70" s="3" t="n"/>
       <c r="U70" s="3" t="n"/>
-      <c r="V70" s="1" t="n"/>
-      <c r="W70" s="1" t="n"/>
-      <c r="X70" s="1" t="n"/>
+      <c r="V70" s="59" t="inlineStr">
+        <is>
+          <t>FME (Lec)</t>
+        </is>
+      </c>
+      <c r="W70" s="43" t="n"/>
+      <c r="X70" s="44" t="n"/>
       <c r="Y70" s="1" t="n"/>
       <c r="Z70" s="1" t="n"/>
       <c r="AA70" s="1" t="n"/>
@@ -4090,7 +4154,7 @@
       <c r="G71" s="44" t="n"/>
       <c r="H71" s="51" t="inlineStr">
         <is>
-          <t>Igor Gaponov</t>
+          <t>Giancarlo Succi</t>
         </is>
       </c>
       <c r="I71" s="43" t="n"/>
@@ -4106,9 +4170,13 @@
       <c r="S71" s="3" t="n"/>
       <c r="T71" s="4" t="n"/>
       <c r="U71" s="4" t="n"/>
-      <c r="V71" s="1" t="n"/>
-      <c r="W71" s="1" t="n"/>
-      <c r="X71" s="1" t="n"/>
+      <c r="V71" s="59" t="inlineStr">
+        <is>
+          <t>Hein Roelfsema</t>
+        </is>
+      </c>
+      <c r="W71" s="43" t="n"/>
+      <c r="X71" s="44" t="n"/>
       <c r="Y71" s="1" t="n"/>
       <c r="Z71" s="1" t="n"/>
       <c r="AA71" s="1" t="n"/>
@@ -4130,7 +4198,7 @@
       <c r="F72" s="43" t="n"/>
       <c r="G72" s="44" t="n"/>
       <c r="H72" s="51" t="n">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I72" s="43" t="n"/>
       <c r="J72" s="43" t="n"/>
@@ -4145,9 +4213,11 @@
       <c r="S72" s="3" t="n"/>
       <c r="T72" s="3" t="n"/>
       <c r="U72" s="3" t="n"/>
-      <c r="V72" s="1" t="n"/>
-      <c r="W72" s="1" t="n"/>
-      <c r="X72" s="1" t="n"/>
+      <c r="V72" s="59" t="n">
+        <v>107</v>
+      </c>
+      <c r="W72" s="43" t="n"/>
+      <c r="X72" s="44" t="n"/>
       <c r="Y72" s="1" t="n"/>
       <c r="Z72" s="1" t="n"/>
       <c r="AA72" s="1" t="n"/>
@@ -4180,7 +4250,7 @@
       <c r="G73" s="44" t="n"/>
       <c r="H73" s="53" t="inlineStr">
         <is>
-          <t>PM (Tut)</t>
+          <t>OS (Tut)</t>
         </is>
       </c>
       <c r="I73" s="43" t="n"/>
@@ -4227,7 +4297,7 @@
       <c r="G74" s="44" t="n"/>
       <c r="H74" s="53" t="inlineStr">
         <is>
-          <t>Semen Kurkin</t>
+          <t>Nikita Lozhnikov</t>
         </is>
       </c>
       <c r="I74" s="43" t="n"/>
@@ -4321,23 +4391,23 @@
         </is>
       </c>
       <c r="G76" s="1" t="n"/>
-      <c r="H76" s="56" t="inlineStr">
-        <is>
-          <t>PM (Lab)</t>
+      <c r="H76" s="55" t="inlineStr">
+        <is>
+          <t>OS (Lab)</t>
         </is>
       </c>
       <c r="I76" s="1" t="n"/>
       <c r="J76" s="53" t="inlineStr">
         <is>
-          <t>PM (Lab)</t>
-        </is>
-      </c>
-      <c r="K76" s="51" t="inlineStr">
-        <is>
-          <t>PS (Lab)</t>
-        </is>
-      </c>
-      <c r="L76" s="1" t="n"/>
+          <t>OS (Lab)</t>
+        </is>
+      </c>
+      <c r="K76" s="1" t="n"/>
+      <c r="L76" s="51" t="inlineStr">
+        <is>
+          <t>OS (Lab)</t>
+        </is>
+      </c>
       <c r="M76" s="1" t="n"/>
       <c r="N76" s="1" t="n"/>
       <c r="O76" s="1" t="n"/>
@@ -4382,21 +4452,21 @@
       <c r="G77" s="1" t="n"/>
       <c r="H77" s="51" t="inlineStr">
         <is>
-          <t>Mikhail Ivanov</t>
+          <t>Nikita Lozhnikov</t>
         </is>
       </c>
       <c r="I77" s="1" t="n"/>
       <c r="J77" s="53" t="inlineStr">
         <is>
-          <t>Victor Nikiforov</t>
-        </is>
-      </c>
-      <c r="K77" s="51" t="inlineStr">
-        <is>
-          <t>Alexey Shikulin</t>
-        </is>
-      </c>
-      <c r="L77" s="1" t="n"/>
+          <t>Xavier Vasquez</t>
+        </is>
+      </c>
+      <c r="K77" s="1" t="n"/>
+      <c r="L77" s="51" t="inlineStr">
+        <is>
+          <t>Shokhista Ergasheva</t>
+        </is>
+      </c>
       <c r="M77" s="3" t="n"/>
       <c r="N77" s="1" t="n"/>
       <c r="O77" s="1" t="n"/>
@@ -4429,7 +4499,7 @@
         <v>102</v>
       </c>
       <c r="E78" s="2" t="n"/>
-      <c r="F78" s="55" t="n">
+      <c r="F78" s="56" t="n">
         <v>103</v>
       </c>
       <c r="G78" s="3" t="n"/>
@@ -4440,10 +4510,10 @@
       <c r="J78" s="53" t="n">
         <v>300</v>
       </c>
-      <c r="K78" s="51" t="n">
+      <c r="K78" s="1" t="n"/>
+      <c r="L78" s="51" t="n">
         <v>301</v>
       </c>
-      <c r="L78" s="1" t="n"/>
       <c r="M78" s="3" t="n"/>
       <c r="N78" s="1" t="n"/>
       <c r="O78" s="1" t="n"/>
@@ -4493,13 +4563,13 @@
       <c r="H79" s="1" t="n"/>
       <c r="I79" s="53" t="inlineStr">
         <is>
-          <t>PM (Lab)</t>
+          <t>OS (Lab)</t>
         </is>
       </c>
       <c r="J79" s="1" t="n"/>
       <c r="K79" s="53" t="inlineStr">
         <is>
-          <t>PM (Lab)</t>
+          <t>OS (Lab)</t>
         </is>
       </c>
       <c r="L79" s="51" t="inlineStr">
@@ -4507,7 +4577,11 @@
           <t>PS (Lab)</t>
         </is>
       </c>
-      <c r="M79" s="3" t="n"/>
+      <c r="M79" s="53" t="inlineStr">
+        <is>
+          <t>OS (Lab)</t>
+        </is>
+      </c>
       <c r="N79" s="1" t="n"/>
       <c r="O79" s="1" t="n"/>
       <c r="P79" s="1" t="n"/>
@@ -4532,19 +4606,19 @@
     <row r="80">
       <c r="A80" s="52" t="n"/>
       <c r="B80" s="6" t="n"/>
-      <c r="C80" s="55" t="inlineStr">
+      <c r="C80" s="56" t="inlineStr">
         <is>
           <t>Vladislav Ostankovich</t>
         </is>
       </c>
       <c r="D80" s="3" t="n"/>
-      <c r="E80" s="55" t="inlineStr">
+      <c r="E80" s="56" t="inlineStr">
         <is>
           <t>Manuel Rodriguez</t>
         </is>
       </c>
       <c r="F80" s="3" t="n"/>
-      <c r="G80" s="55" t="inlineStr">
+      <c r="G80" s="56" t="inlineStr">
         <is>
           <t>Hamza Salem</t>
         </is>
@@ -4552,13 +4626,13 @@
       <c r="H80" s="1" t="n"/>
       <c r="I80" s="53" t="inlineStr">
         <is>
-          <t>Mikhail Ivanov</t>
+          <t>Nikita Lozhnikov</t>
         </is>
       </c>
       <c r="J80" s="1" t="n"/>
       <c r="K80" s="53" t="inlineStr">
         <is>
-          <t>Victor Nikiforov</t>
+          <t>Xavier Vasquez</t>
         </is>
       </c>
       <c r="L80" s="51" t="inlineStr">
@@ -4566,7 +4640,11 @@
           <t>Alexey Shikulin</t>
         </is>
       </c>
-      <c r="M80" s="3" t="n"/>
+      <c r="M80" s="53" t="inlineStr">
+        <is>
+          <t>Shokhista Ergasheva</t>
+        </is>
+      </c>
       <c r="N80" s="1" t="n"/>
       <c r="O80" s="1" t="n"/>
       <c r="P80" s="1" t="n"/>
@@ -4611,9 +4689,11 @@
         <v>300</v>
       </c>
       <c r="L81" s="51" t="n">
+        <v>302</v>
+      </c>
+      <c r="M81" s="53" t="n">
         <v>301</v>
       </c>
-      <c r="M81" s="3" t="n"/>
       <c r="N81" s="1" t="n"/>
       <c r="O81" s="1" t="n"/>
       <c r="P81" s="1" t="n"/>
@@ -5019,7 +5099,7 @@
       <c r="G92" s="44" t="n"/>
       <c r="H92" s="51" t="inlineStr">
         <is>
-          <t>DE (Lec)</t>
+          <t>PM (Lec)</t>
         </is>
       </c>
       <c r="I92" s="43" t="n"/>
@@ -5031,14 +5111,26 @@
       <c r="O92" s="3" t="n"/>
       <c r="P92" s="3" t="n"/>
       <c r="Q92" s="3" t="n"/>
-      <c r="R92" s="3" t="n"/>
-      <c r="S92" s="3" t="n"/>
-      <c r="T92" s="3" t="n"/>
-      <c r="U92" s="3" t="n"/>
+      <c r="R92" s="57" t="inlineStr">
+        <is>
+          <t>P2 (Lec)</t>
+        </is>
+      </c>
+      <c r="S92" s="44" t="n"/>
+      <c r="T92" s="60" t="inlineStr">
+        <is>
+          <t>CV (Lec)</t>
+        </is>
+      </c>
+      <c r="U92" s="44" t="n"/>
       <c r="V92" s="1" t="n"/>
       <c r="W92" s="1" t="n"/>
       <c r="X92" s="1" t="n"/>
-      <c r="Y92" s="1" t="n"/>
+      <c r="Y92" s="59" t="inlineStr">
+        <is>
+          <t>CV (Lec)</t>
+        </is>
+      </c>
       <c r="Z92" s="1" t="n"/>
       <c r="AA92" s="1" t="n"/>
       <c r="AB92" s="1" t="n"/>
@@ -5062,7 +5154,7 @@
       <c r="G93" s="44" t="n"/>
       <c r="H93" s="51" t="inlineStr">
         <is>
-          <t>Nikolay Shilov</t>
+          <t>Igor Gaponov</t>
         </is>
       </c>
       <c r="I93" s="43" t="n"/>
@@ -5074,14 +5166,26 @@
       <c r="O93" s="3" t="n"/>
       <c r="P93" s="3" t="n"/>
       <c r="Q93" s="3" t="n"/>
-      <c r="R93" s="3" t="n"/>
-      <c r="S93" s="3" t="n"/>
-      <c r="T93" s="4" t="n"/>
-      <c r="U93" s="4" t="n"/>
+      <c r="R93" s="57" t="inlineStr">
+        <is>
+          <t>Artur Karimov</t>
+        </is>
+      </c>
+      <c r="S93" s="44" t="n"/>
+      <c r="T93" s="61" t="inlineStr">
+        <is>
+          <t>Mohamed Fahim</t>
+        </is>
+      </c>
+      <c r="U93" s="44" t="n"/>
       <c r="V93" s="1" t="n"/>
       <c r="W93" s="1" t="n"/>
       <c r="X93" s="1" t="n"/>
-      <c r="Y93" s="1" t="n"/>
+      <c r="Y93" s="59" t="inlineStr">
+        <is>
+          <t>Mohamed Fahim</t>
+        </is>
+      </c>
       <c r="Z93" s="1" t="n"/>
       <c r="AA93" s="1" t="n"/>
       <c r="AB93" s="1" t="n"/>
@@ -5102,7 +5206,7 @@
       <c r="F94" s="43" t="n"/>
       <c r="G94" s="44" t="n"/>
       <c r="H94" s="51" t="n">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="I94" s="43" t="n"/>
       <c r="J94" s="43" t="n"/>
@@ -5113,14 +5217,20 @@
       <c r="O94" s="3" t="n"/>
       <c r="P94" s="3" t="n"/>
       <c r="Q94" s="3" t="n"/>
-      <c r="R94" s="3" t="n"/>
-      <c r="S94" s="3" t="n"/>
-      <c r="T94" s="3" t="n"/>
-      <c r="U94" s="3" t="n"/>
+      <c r="R94" s="57" t="n">
+        <v>106</v>
+      </c>
+      <c r="S94" s="44" t="n"/>
+      <c r="T94" s="60" t="n">
+        <v>108</v>
+      </c>
+      <c r="U94" s="44" t="n"/>
       <c r="V94" s="1" t="n"/>
       <c r="W94" s="1" t="n"/>
       <c r="X94" s="1" t="n"/>
-      <c r="Y94" s="1" t="n"/>
+      <c r="Y94" s="59" t="n">
+        <v>108</v>
+      </c>
       <c r="Z94" s="1" t="n"/>
       <c r="AA94" s="1" t="n"/>
       <c r="AB94" s="1" t="n"/>
@@ -5148,7 +5258,7 @@
       <c r="G95" s="44" t="n"/>
       <c r="H95" s="53" t="inlineStr">
         <is>
-          <t>DE (Tut)</t>
+          <t>PM (Tut)</t>
         </is>
       </c>
       <c r="I95" s="43" t="n"/>
@@ -5191,7 +5301,7 @@
       <c r="G96" s="44" t="n"/>
       <c r="H96" s="53" t="inlineStr">
         <is>
-          <t>Ivan Konyukhov</t>
+          <t>Semen Kurkin</t>
         </is>
       </c>
       <c r="I96" s="43" t="n"/>
@@ -5223,7 +5333,7 @@
     <row r="97">
       <c r="A97" s="48" t="n"/>
       <c r="B97" s="54" t="n">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C97" s="43" t="n"/>
       <c r="D97" s="43" t="n"/>
@@ -5231,7 +5341,7 @@
       <c r="F97" s="43" t="n"/>
       <c r="G97" s="44" t="n"/>
       <c r="H97" s="53" t="n">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I97" s="43" t="n"/>
       <c r="J97" s="43" t="n"/>
@@ -5283,23 +5393,19 @@
       </c>
       <c r="F98" s="1" t="n"/>
       <c r="G98" s="1" t="n"/>
-      <c r="H98" s="56" t="inlineStr">
-        <is>
-          <t>DE (Lab)</t>
+      <c r="H98" s="55" t="inlineStr">
+        <is>
+          <t>PM (Lab)</t>
         </is>
       </c>
       <c r="I98" s="1" t="n"/>
       <c r="J98" s="53" t="inlineStr">
         <is>
-          <t>DE (Lab)</t>
+          <t>PM (Lab)</t>
         </is>
       </c>
       <c r="K98" s="1" t="n"/>
-      <c r="L98" s="51" t="inlineStr">
-        <is>
-          <t>PM (Lab)</t>
-        </is>
-      </c>
+      <c r="L98" s="1" t="n"/>
       <c r="M98" s="1" t="n"/>
       <c r="N98" s="1" t="n"/>
       <c r="O98" s="1" t="n"/>
@@ -5344,21 +5450,17 @@
       <c r="G99" s="1" t="n"/>
       <c r="H99" s="51" t="inlineStr">
         <is>
-          <t>Marat Mingazov</t>
+          <t>Mikhail Ivanov</t>
         </is>
       </c>
       <c r="I99" s="1" t="n"/>
       <c r="J99" s="53" t="inlineStr">
         <is>
-          <t>Victor Kazorin</t>
+          <t>Victor Nikiforov</t>
         </is>
       </c>
       <c r="K99" s="1" t="n"/>
-      <c r="L99" s="51" t="inlineStr">
-        <is>
-          <t>Victor Nikiforov</t>
-        </is>
-      </c>
+      <c r="L99" s="1" t="n"/>
       <c r="M99" s="3" t="n"/>
       <c r="N99" s="1" t="n"/>
       <c r="O99" s="1" t="n"/>
@@ -5384,28 +5486,26 @@
     <row r="100">
       <c r="A100" s="48" t="n"/>
       <c r="B100" s="49" t="n">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C100" s="50" t="n">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D100" s="2" t="n"/>
       <c r="E100" s="50" t="n">
-        <v>300</v>
+        <v>103</v>
       </c>
       <c r="F100" s="3" t="n"/>
       <c r="G100" s="3" t="n"/>
       <c r="H100" s="51" t="n">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="I100" s="1" t="n"/>
       <c r="J100" s="53" t="n">
-        <v>102</v>
+        <v>300</v>
       </c>
       <c r="K100" s="1" t="n"/>
-      <c r="L100" s="51" t="n">
-        <v>301</v>
-      </c>
+      <c r="L100" s="1" t="n"/>
       <c r="M100" s="3" t="n"/>
       <c r="N100" s="1" t="n"/>
       <c r="O100" s="1" t="n"/>
@@ -5455,21 +5555,17 @@
       <c r="H101" s="1" t="n"/>
       <c r="I101" s="53" t="inlineStr">
         <is>
-          <t>DE (Lab)</t>
+          <t>PM (Lab)</t>
         </is>
       </c>
       <c r="J101" s="1" t="n"/>
       <c r="K101" s="53" t="inlineStr">
         <is>
-          <t>DE (Lab)</t>
+          <t>PM (Lab)</t>
         </is>
       </c>
       <c r="L101" s="1" t="n"/>
-      <c r="M101" s="53" t="inlineStr">
-        <is>
-          <t>PM (Lab)</t>
-        </is>
-      </c>
+      <c r="M101" s="3" t="n"/>
       <c r="N101" s="1" t="n"/>
       <c r="O101" s="1" t="n"/>
       <c r="P101" s="1" t="n"/>
@@ -5495,18 +5591,18 @@
       <c r="A102" s="52" t="n"/>
       <c r="B102" s="6" t="n"/>
       <c r="C102" s="3" t="n"/>
-      <c r="D102" s="55" t="inlineStr">
+      <c r="D102" s="56" t="inlineStr">
         <is>
           <t>Naumcheva Mariya</t>
         </is>
       </c>
       <c r="E102" s="3" t="n"/>
-      <c r="F102" s="55" t="inlineStr">
+      <c r="F102" s="56" t="inlineStr">
         <is>
           <t>Ilya Khomyakov</t>
         </is>
       </c>
-      <c r="G102" s="55" t="inlineStr">
+      <c r="G102" s="56" t="inlineStr">
         <is>
           <t>Ruzilia Mukhutdinova</t>
         </is>
@@ -5514,21 +5610,17 @@
       <c r="H102" s="1" t="n"/>
       <c r="I102" s="53" t="inlineStr">
         <is>
-          <t>Marat Mingazov</t>
+          <t>Mikhail Ivanov</t>
         </is>
       </c>
       <c r="J102" s="1" t="n"/>
       <c r="K102" s="53" t="inlineStr">
         <is>
-          <t>Victor Kazorin</t>
+          <t>Victor Nikiforov</t>
         </is>
       </c>
       <c r="L102" s="1" t="n"/>
-      <c r="M102" s="53" t="inlineStr">
-        <is>
-          <t>Victor Nikiforov</t>
-        </is>
-      </c>
+      <c r="M102" s="3" t="n"/>
       <c r="N102" s="1" t="n"/>
       <c r="O102" s="1" t="n"/>
       <c r="P102" s="1" t="n"/>
@@ -5555,27 +5647,25 @@
       <c r="B103" s="5" t="n"/>
       <c r="C103" s="1" t="n"/>
       <c r="D103" s="50" t="n">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E103" s="1" t="n"/>
       <c r="F103" s="50" t="n">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G103" s="50" t="n">
-        <v>300</v>
+        <v>103</v>
       </c>
       <c r="H103" s="1" t="n"/>
       <c r="I103" s="53" t="n">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="J103" s="1" t="n"/>
       <c r="K103" s="53" t="n">
-        <v>102</v>
+        <v>300</v>
       </c>
       <c r="L103" s="1" t="n"/>
-      <c r="M103" s="53" t="n">
-        <v>301</v>
-      </c>
+      <c r="M103" s="3" t="n"/>
       <c r="N103" s="1" t="n"/>
       <c r="O103" s="1" t="n"/>
       <c r="P103" s="1" t="n"/>
@@ -5615,7 +5705,7 @@
       <c r="K104" s="1" t="n"/>
       <c r="L104" s="53" t="inlineStr">
         <is>
-          <t>DE (Lab)</t>
+          <t>PM (Lab)</t>
         </is>
       </c>
       <c r="M104" s="1" t="n"/>
@@ -5654,7 +5744,7 @@
       <c r="K105" s="1" t="n"/>
       <c r="L105" s="53" t="inlineStr">
         <is>
-          <t>Marat Mingazov</t>
+          <t>Victor Nikiforov</t>
         </is>
       </c>
       <c r="M105" s="1" t="n"/>
@@ -5735,7 +5825,7 @@
       <c r="L107" s="1" t="n"/>
       <c r="M107" s="51" t="inlineStr">
         <is>
-          <t>DE (Lab)</t>
+          <t>PM (Lab)</t>
         </is>
       </c>
       <c r="N107" s="1" t="n"/>
@@ -5774,7 +5864,7 @@
       <c r="L108" s="1" t="n"/>
       <c r="M108" s="51" t="inlineStr">
         <is>
-          <t>Marat Mingazov</t>
+          <t>Victor Nikiforov</t>
         </is>
       </c>
       <c r="N108" s="1" t="n"/>
@@ -5967,7 +6057,7 @@
     <row r="133"/>
     <row r="134"/>
   </sheetData>
-  <mergeCells count="123">
+  <mergeCells count="141">
     <mergeCell ref="A10:A12"/>
     <mergeCell ref="A7:A9"/>
     <mergeCell ref="A4:A6"/>
@@ -6037,54 +6127,72 @@
     <mergeCell ref="F73:G73"/>
     <mergeCell ref="F74:G74"/>
     <mergeCell ref="F75:G75"/>
+    <mergeCell ref="T92:U92"/>
+    <mergeCell ref="T93:U93"/>
+    <mergeCell ref="T94:U94"/>
+    <mergeCell ref="Y92"/>
+    <mergeCell ref="Y93"/>
+    <mergeCell ref="Y94"/>
+    <mergeCell ref="H4:M4"/>
+    <mergeCell ref="H5:M5"/>
+    <mergeCell ref="H6:M6"/>
+    <mergeCell ref="H7:M7"/>
+    <mergeCell ref="H8:M8"/>
+    <mergeCell ref="H9:M9"/>
+    <mergeCell ref="B92:G92"/>
+    <mergeCell ref="B93:G93"/>
+    <mergeCell ref="B94:G94"/>
+    <mergeCell ref="B95:G95"/>
+    <mergeCell ref="B96:G96"/>
+    <mergeCell ref="B97:G97"/>
+    <mergeCell ref="N26:R26"/>
+    <mergeCell ref="N27:R27"/>
+    <mergeCell ref="N28:R28"/>
+    <mergeCell ref="Z48:AA48"/>
+    <mergeCell ref="Z49:AA49"/>
+    <mergeCell ref="Z50:AA50"/>
+    <mergeCell ref="V70:X70"/>
+    <mergeCell ref="V71:X71"/>
+    <mergeCell ref="V72:X72"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="H48:M48"/>
+    <mergeCell ref="H49:M49"/>
+    <mergeCell ref="H50:M50"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F48:G48"/>
+    <mergeCell ref="F49:G49"/>
+    <mergeCell ref="F50:G50"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="F52:G52"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="H70:M70"/>
+    <mergeCell ref="H71:M71"/>
+    <mergeCell ref="H72:M72"/>
+    <mergeCell ref="H73:M73"/>
+    <mergeCell ref="H74:M74"/>
+    <mergeCell ref="H75:M75"/>
+    <mergeCell ref="R92:S92"/>
+    <mergeCell ref="R93:S93"/>
+    <mergeCell ref="R94:S94"/>
     <mergeCell ref="H92:M92"/>
     <mergeCell ref="H93:M93"/>
     <mergeCell ref="H94:M94"/>
     <mergeCell ref="H95:M95"/>
     <mergeCell ref="H96:M96"/>
     <mergeCell ref="H97:M97"/>
-    <mergeCell ref="B92:G92"/>
-    <mergeCell ref="B93:G93"/>
-    <mergeCell ref="B94:G94"/>
-    <mergeCell ref="B95:G95"/>
-    <mergeCell ref="B96:G96"/>
-    <mergeCell ref="B97:G97"/>
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="H4:M4"/>
-    <mergeCell ref="H5:M5"/>
-    <mergeCell ref="H6:M6"/>
-    <mergeCell ref="F48:G48"/>
-    <mergeCell ref="F49:G49"/>
-    <mergeCell ref="F50:G50"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="F52:G52"/>
-    <mergeCell ref="F53:G53"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="H26:M26"/>
-    <mergeCell ref="H27:M27"/>
-    <mergeCell ref="H28:M28"/>
-    <mergeCell ref="H29:M29"/>
-    <mergeCell ref="H30:M30"/>
-    <mergeCell ref="H31:M31"/>
-    <mergeCell ref="H70:M70"/>
-    <mergeCell ref="H71:M71"/>
-    <mergeCell ref="H72:M72"/>
-    <mergeCell ref="H73:M73"/>
-    <mergeCell ref="H74:M74"/>
-    <mergeCell ref="H75:M75"/>
-    <mergeCell ref="H48:M48"/>
-    <mergeCell ref="H49:M49"/>
-    <mergeCell ref="H50:M50"/>
-    <mergeCell ref="H51:M51"/>
-    <mergeCell ref="H52:M52"/>
-    <mergeCell ref="H53:M53"/>
+    <mergeCell ref="H32:M32"/>
+    <mergeCell ref="H33:M33"/>
+    <mergeCell ref="H34:M34"/>
+    <mergeCell ref="H35:M35"/>
+    <mergeCell ref="H36:M36"/>
+    <mergeCell ref="H37:M37"/>
     <mergeCell ref="B32:E32"/>
     <mergeCell ref="B33:E33"/>
     <mergeCell ref="B34:E34"/>

</xml_diff>